<commit_message>
Get daily reddit data: Tue Nov 12 08:10:47 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_17.xlsx
+++ b/data/collected_data/2024_11_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C489"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,3202 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1gpfvfb</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What can do with this, help </t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ogxvyqa9hf0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1gpfkja</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Best nail hardening and nourishing polish?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpfkja/best_nail_hardening_and_nourishing_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1gpf7p7</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>new to this and having fun!</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpf7p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1gpd0tl</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Broke a nail the DAY AFTER getting a manicure 😭 (my fault or no?)</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpd0tl/broke_a_nail_the_day_after_getting_a_manicure_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1gpeync</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>birthday nails!</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yxqcms45f0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1gpekr0</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>help 😭 WORST nails ever.</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpekr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1gpdtp5</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Nails I did for the Military Ball this year</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpdtp5</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1gpcg71</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Christmas, snow, winter themed etc nails ⛸️❄️😍</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpcg71/christmas_snow_winter_themed_etc_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1gpcwiq</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>What are your thoughts?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqd1nsskhe0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1gpcoky</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">sHiNy or mAtTe ?? </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpcoky</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1gpcjg1</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Concert themed nails </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpcjg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1gpbx2k</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>it’s been a while 🩶</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpbx2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1gpbsoa</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Coraline Nails</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpbsoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1gpbm5e</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So happy with these. Can’t wait to add some little hearts </t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shlwp1tw4e0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1gpbh5z</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frozen 🥶 </t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlzq60bk3e0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1gpbc4c</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Simple and short is the way I like it</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wu8r1082e0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1gpax0d</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Short velvet snowflake nails with crystals ❄️</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpax0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1gpasyt</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Loving this shade of red 🍒</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42jewlz7xd0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1gp9yde</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>💚💙🖤🤍</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvtpfxbkpd0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1gp9sp5</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really like how my nails turned out </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekswdzw6od0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1gp9n9h</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Practice makes perfect🙈 </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp9n9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1gp9nz7</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oooh, glitter! </t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp9nz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1gp98os</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying press-ons after natural nails broke </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z70vw6f7jd0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1gp8lj5</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Urgent call to all my nail art Kings and Queens! </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp8lj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1gp8i7i</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>I did a thing (second try)</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp8i7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1gp84qh</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Wanted something simple for fall. Turned out great!</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eayzexhs9d0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1gp7t9n</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>What nail polish brands are worth ordering online? (Colour range, durability. etc)</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gp7t9n/what_nail_polish_brands_are_worth_ordering_online/</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1gp7rl7</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Hello beautiful people. I do my nails every month and my question is: should I rest at some point? now it's time for service as you will see</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cklbl5sq6d0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1gp7che</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>why do people do this 🥲</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jiebdl83d0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1gp673l</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Hard Gel Ex and that bloody electric file</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gp673l/hard_gel_ex_and_that_bloody_electric_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1gp6xiz</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>My first try at sweater nails :)</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp6xiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1gp6rfj</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Is it just me or is white acrylic hard to work with?</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gp6rfj/is_it_just_me_or_is_white_acrylic_hard_to_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1gp6pac</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Does anybody else feel like your fingers are actually toes when you go bare after years of having the strongest, longest dip &amp; gel painted nails?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvz26qa1yc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1gp6os0</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>I’m loving the color. 💜☮️</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evub92wwxc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1gp6ok7</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybpekvivxc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1gp6dfe</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Can I file my nails after a gel overlay?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6lvtpfdvc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1gp6cl0</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>platinum chrome</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/am6e88s7vc0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1gp63iu</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Fave nails I've done</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eofupy3atc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1gp5x24</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Should I ask my nail tech to fix?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cywal6uyrc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1gp5q88</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help. Press-ons do not fit. </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5t99x1fiqc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1gp5bjt</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted JoJos nails by me ⭐️ </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/slbxmzdfnc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1gp4ylz</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>My favorite manicure. What do you think?</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4g44mjfnkc0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1gp4cs1</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kuromi &amp; My Melody set </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6ssgng47gc0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1gp46s3</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>My nails burned badly the last time I got them done and now I’m scared</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gp46s3/my_nails_burned_badly_the_last_time_i_got_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1gp48yn</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"pure" by ella + mila </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp48yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1gp3apr</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>I loved this effect!!</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58rrgu4h8c0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1gp31l5</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Coming into Winter with a breeze</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3faq5ugo6c0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1gp2kyv</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Any tips for preventing gel allergy?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gp2kyv/any_tips_for_preventing_gel_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1gp2o4w</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Halloween press ons</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n05vl5tw3c0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1gp2mb3</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Best Flash Cure Lamp</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gp2mb3/best_flash_cure_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1gp2m3t</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Flame on!</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp2m3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1gp2l7s</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First two shaping attempts </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep1sbb1b3c0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1gp2h73</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press On Brand Recommendations </t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jh1vexi2c0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1gp2dga</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Light milky ombre</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ih3l6f3h1c0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1gp1ru0</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>How to deal with crooked / tilted nails, nailbeds or fingers? (Image is just illustrative)</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gp9kurlxb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1gp1oaj</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>How to remove builder gel without drill</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gp1oaj/how_to_remove_builder_gel_without_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1gp1kn2</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing builder gel </t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cps5r7d6wb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1gp1be1</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">green and purple </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp1be1</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1gp0l5f</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Chocolate Plum for Late Autumn</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dc6lihr0pb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1gp0a8n</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cinderella Nails </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp0a8n</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1gp03n5</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Blink-182 Album Art Nails</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiyhd8rhlb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1gp01sx</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Absolutely OBSESSED with this dreamy chrome combo</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp01sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1gozilh</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>I’ve had these nails for a week. I’ve never had so many people compliment /ask to take inspiration pics!</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shn68o8fhb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1gozm74</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>A set I did recently ✨🫧🌟</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gozm74</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1gozbab</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Gel extensions nails not lasting as long as acrylic?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gozbab/gel_extensions_nails_not_lasting_as_long_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1gozagh</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Easing into fall</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gozagh</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1goz1nn</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>White line is weird??</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goz1nn</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1goz6lh</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Remove nails</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1goz6lh/remove_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1goyxvj</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 14yr olds very first set ever! </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goyxvj</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1goychz</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Made these press ons for my grandma’s first concert in 30 years 🥹</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goychz</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1goybaf</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Finally hopped on the tortoise shell trend</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrdq35jw8b0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1goy663</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Late photo of my Halloween set. 🐈‍⬛ 💀 👻 </t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goy663</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1goxrhc</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I was inspired by all the mirror chromes I've been seeing lately so I took silver, gold and red and mixed silver and red and gold and red. </t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23ldz2cx4b0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1gowxay</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Olive &amp; June Review!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eimtjl44za0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1goxplo</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Autumn shades</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goxplo</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1goxkkk</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Loooove! 💛</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h8fqistl3b0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1goxirw</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>What about tiny nails?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goxirw</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1goww7l</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>I just wanted to show my "Nakey Nails" all prepped and ready for Nail Day today</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goww7l</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1gowqun</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>🥰</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jal03gdwxa0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1gowpod</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Sweater nail design 💕</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g71whdqnxa0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1gowj5b</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Can I file these on my own?</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8x2rjl1cwa0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1govxn5</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Press on Sizing</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/acv7if0xra0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1goo42a</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Broken nails from gel extensions</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9xvvwwhn80e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1gouyfa</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Burgundy nailss </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5v1l1mkka0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1gouurh</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Is this flattering for me?😬</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hdeqmsttja0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1gouaga</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Jojoba Oil Causing More Hangnails?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gouaga/jojoba_oil_causing_more_hangnails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1gou1qu</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Milky white with a soft pearl chrome on top of builder gel</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gou1qu</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1gottdn</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Sorry if this is a dumb/repetitive topic...🥲</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gottdn/sorry_if_this_is_a_dumbrepetitive_topic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1gotj6t</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Birthday treat to myself. First time getting French tips!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/554nfz0m9a0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1got7m9</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>One week of growth, send help lol</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/op729i907a0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1got3xk</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>French tip I did myself! Those nail stampers work 🙌</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1got3xk</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1goskit</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Bedazzled press ons✨</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goskit</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1gos81c</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>new nails, new mood.</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/stxv827ay90e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1gorx2y</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I don’t know about these press ons </t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i99s5tyqv90e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1gopi9c</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>UV light BURNED 🔥</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vp94rtou590e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1gordgc</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>my second set ever</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gordgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1gor8gv</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kiss gel x-tend </t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gor8gv</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1gor61v</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>They are beautiful, I am enchanted.</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52o0d9fmo90e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1goqvlz</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Weir creatures </t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goqvlz</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1goqp8p</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Permission granted</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e2cuziznj90e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1gpfapj</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Stop thinners damaging nails?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpfapj/stop_thinners_damaging_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1gpe0ml</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Bees Knees Elden Ring!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oc3nnchjte0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1gpcxtx</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Broke a nail the DAY AFTER getting a manicure 😭 (my fault or no?)</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e39j5xuxhe0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1gpc9gw</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Tips &amp; Regular Polish?? Need advice!</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpc9gw/tips_regular_polish_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1gpc4a8</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Polishes that look like opals?</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpc4a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1gpbodq</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Is gel magnetic stronger than regular polish??</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpbodq/is_gel_magnetic_stronger_than_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1gpbm14</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>The magic of Sech Vive self-leveling y'all...</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpbm14</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1gpb8u0</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Terracotta shade </t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpb8u0/terracotta_shade/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1gpaw8o</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Sally's insta dry Back to Black and Holo-Back</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wg6prl2yd0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1gpaqsp</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Forget Me Not topped with Let it Glow (blue) from Fancy Gloss</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d44077gjwd0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1gpaoxk</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Wet Polish is prettier?</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpaoxk/wet_polish_is_prettier/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1gpa8zj</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Curious question about gel allergery</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpa8zj/curious_question_about_gel_allergery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1gpa72j</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Favorite nail primers for an even canvas?</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpa72j/favorite_nail_primers_for_an_even_canvas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1gpa4i9</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Cirque Coronation</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpa4i9/cirque_coronation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1gp9xm6</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Fall leaves inspired mani 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kv1lndfdpd0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1gp921h</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Does anyone know what kind of magnet / technique was used to achieve the effect seen on these swatch pictures for Clionadh Cosmetics' Psilocybin?</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp921h</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1gp908l</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>anybody know where to get these?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phqsz5g7hd0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1gp7y6n</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Accent nail(s), yay or nay?</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gp7y6n/accent_nails_yay_or_nay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1gp7rya</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Red Swatches</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp7rya</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1gp6nqy</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>small but mighty holiday haul 🎄</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyaj6jgpxc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1gp6dum</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Warm skittles? For autumn? Groundbreaking. </t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtk623oivc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1gp5tt8</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Kokie “Knockout” - vibrant royal purple 😍💜</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp5tt8</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1gp5b1n</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Please rate my first professional mani</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2zfipzbnc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1gp57o7</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Monarch and speckled wood butterfly inspired nails</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp57o7</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1gp564z</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>First set in over a year!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lamcv3hamc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1gp4xl8</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Sassy sauce black Friday release</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp4xl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1gp4qtr</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>metallic polishes without sparkles/shimmer?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gp4qtr/metallic_polishes_without_sparklesshimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1gp4mzo</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Loved this result 🩷✨️</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72rqorqcic0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1gp4h1m</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Chocolate Fever 🍫🌡</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp4h1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1gp45pb</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>This is from a 2022 article about DIY pedicures. Oxygenating your nails? Really?</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzq2ciemec0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1gp40u5</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>What is your favorite guide for using nail polish thinner?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gp40u5/what_is_your_favorite_guide_for_using_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1gp3uev</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Gel spilled onto my finger now what?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cazs3sfcc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1gp3q07</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>What’s the deal with the Cirque Colors Facebook group?</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gp3q07/whats_the_deal_with_the_cirque_colors_facebook/</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1gp3ltk</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Perfect season for Hot Toddy</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp3ltk</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1gp3fnc</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>New nail polish, says to blow dry?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp3fnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1gp3931</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Gummy nail polish</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gp3931/gummy_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1gp2yi7</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Anyone have ILNP/Cirque/Drugstore dupes for these?</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.mooncat.com/products/memento-mori</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1gp2vy2</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>LynB swatch request</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gp2vy2/lynb_swatch_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1gp2vjx</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Fall Nails </t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp2vjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1gp1v8d</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>⛅</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp1v8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1gp188f</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Come Again</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp188f</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1gp13gr</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frosty fall nails since it's already showed where I live. </t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp13gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1gp00il</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP color match request </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gp00il/ilnp_color_match_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1gozjlm</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>A hopeful mani</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/98i2hfdmhb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1gozcm9</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Sand viper so snipey</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6a46j28gb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1goyexo</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Feeling Fall</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odso06gm9b0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1goy8xu</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Is this Dam’s “Twinning”?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goy8xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1gox7rh</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Fun fall mani</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gox7rh</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1gox4db</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>the muted red of my dreams</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dre7qk3f0b0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1gox1cn</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Lights Lacquer - Strawberry Boba</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gox1cn</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1gowpcd</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>ILNP - sea glass</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9h3tpdclxa0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1gowl4o</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Why won't my gel polish last?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gowl4o</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1gow1mn</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Gel polish steamer</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gow1mn/gel_polish_steamer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1govzfz</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>The Autumn Blues 💙</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1govzfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1gou7nn</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Does anyone have a comparison of Holo Taco's Never Tide Down vs Mooncat's River Styx?</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gou7nn/does_anyone_have_a_comparison_of_holo_tacos_never/</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1goto3r</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Cirque Magnetics?</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goto3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1gosuoh</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>ILNP - Riddle Me This</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8m64z1ty3a0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1gosavn</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Marsala jelly with some extra sparkles ✨️</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dp7m8ax5z90e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1gos41k</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>One of my favourite polishes atm, EdM - Wished for Tomorrow</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gos41k</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1gorv70</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Accidental dupe ilnp flicker</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gorv70</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1goqwqb</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Marshall's OPI score</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goqwqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1goquc9</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🎼 “Always Coca-Cola” 🎶 </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvmsyit8l90e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1goq3ne</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Magical fairy combo🧚</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goq3ne</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1gopojn</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gopojn/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1gopc81</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Polish Recommendations </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gopc81/gel_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1go3rij</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Can you develop acrylate allergies from new Mylee formula?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1go3rij/can_you_develop_acrylate_allergies_from_new_mylee/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1goj5jk</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Shimmer polish for chocolate brown mani</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1goj5jk/shimmer_polish_for_chocolate_brown_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1gpezvb</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>My favorite set of 2024✨ what do you think?</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8txaecil5f0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1gpbmkq</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Easing into Fall</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpbmkq</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1gp7ufs</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails I did </t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yajr7poe7d0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1gp7bqx</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Alice in wonderland</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp7bqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1gp720d</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I do this kind of nails? </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x7q72ukv0d0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1gp4ekt</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute Kuromi &amp; My Melody </t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ira3qexkgc0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1gp4c4m</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cappuccino! </t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ny1rdnu3gc0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1gp3jtf</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>What do u think?❤️‍🩹</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gp3jtf</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1gp0es5</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>My friend gave me these</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jwia0rqnb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1gp09kf</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Opinions.... 🖤</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qf229zuomb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1gozcwf</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Coca-Cola Santa and Olaf nails  for Christmas!</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gozcwf</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1goysfl</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Powerpuff Girls 🥰</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpin1d98cb0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1goy9m4</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>My Cruella inspired nails</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3a83watk8b0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1goxs79</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Autumn shades</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goxs79</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1gowoqn</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Sweater nail design 💕</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45xix5vgxa0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1gou7fv</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Twilight Inspired Nails🫶🏼</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjcsezfyea0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1gotr39</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Ideal color and design</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ve3txxcba0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1gotft0</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>My sister's moons and stars</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gotft0</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1goom7b</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>I haven't posted in a while but I just love this set I did yesterday and I want to share it</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goom7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1goo7xz</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neon cobra inspired by Tino Vo. </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goo7xz</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1goo3xb</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Another try at this. Brides nails for winter wedding</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1goo3xb</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Nov 13 08:10:38 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_17.xlsx
+++ b/data/collected_data/2024_11_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C489"/>
+  <dimension ref="A1:C681"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8747,6 +8747,3270 @@
         </is>
       </c>
     </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1gq7xan</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Pearly pink glitter gradient 💕</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjfzz34ikm0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1gq7k0n</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Baby Blue 🩵</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5h8yi4efm0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1gq7cn7</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>These were my Halloween nails!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6ukyztvcm0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1gq77eb</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Maybe a little too picnicy for the weather but I couldn’t resist</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ma79bkyam0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1gq6p99</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red nails 💅🏽 </t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxtdq1wp4m0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1gq64bh</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Do my nails look professional?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufl0mr5txl0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1gq5xrp</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>What’s going on with my acrylics ?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2qcddgrvl0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1gq5zmx</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Cyberpunk!</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzmrxstdwl0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1gq5glx</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">45 year old husband - acrylic nails update.   </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq5glx</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1gq4ul1</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Painting a Jinx Nail set and this is me 5 hours in 🫠🥲</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yxrg7h8kl0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1gq4hi2</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out press ons </t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq4hi2</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1gq4au5</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Olive martini nails 🍸</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vl8fzquoel0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1gq3w3u</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Tip snapped off after 1 day. Is something wrong with the application of these acrylic nails?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hsl0yyjnal0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1gq3b9y</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Nail lamp</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gq3b9y/nail_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1gq2xzs</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Accidentally got gel polish on my skin.</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gq2xzs/accidentally_got_gel_polish_on_my_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1gq32z5</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Oh how I love Holo Taco</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq32z5</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1gq32te</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>IT’S HAPPENING!!!!!</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwhxw3753l0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1gq324r</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Combo set 🥰</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq324r</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1gq2m6l</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Colors by Llarowe Berries in the snow</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iba8mqfvyk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1gq29yf</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>first holiday set of the season❄️</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/leutu3ysvk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1gq1jfi</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving Tortoise </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iordtmx8pk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1gq1h6w</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Happy lil flowers!</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oo16uq7pok0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1gq0tzw</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Craziest set I’ve gotten to date</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ruiwfkm1jk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1gq0iki</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>birthday nails XD 🌀</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb32932egk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1gq0htk</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Help with product question!</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gq0htk/help_with_product_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1gq0g5r</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>🦋Fresh Blue Mani🦋</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq0g5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1gq05hm</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black french With pink tips… i think they’re cool. What do you think? </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqel0dkadk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1gq04e8</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Chick Flick Cherry - My dream fall red ☺️</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq04e8</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1gq04dr</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>I know I’m late but I had to post my Halloween set. I was obsessed😍</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7zxi0ve2dk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1gpxx74</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Was this a normal nail salon experience?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpxx74/was_this_a_normal_nail_salon_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1gpz7e9</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Do I need to buff the top before I paint these?</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpz7e9/do_i_need_to_buff_the_top_before_i_paint_these/</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1gpyxy3</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>She killed that once again 💜🤍💙</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpyxy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1gpyr2a</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>i did my own nails for fall!</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yzqmqh2r1k0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1gpydor</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Hand painted Hunter X Hunter nailzzz by me!</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpydor</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1gpxoal</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sweater nails </t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpxoal</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1gpxkvv</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>BIAB Russian Manicure Prices</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqy0q1zdsj0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1gpxjyx</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I dont get my nails dont a lot but this looks bad right </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpxjyx</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1gpxaw5</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Last set before Chrissy nails!</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k98hc269qj0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1gpx8fu</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Four hours later..😑</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpx8fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1gpx1ct</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Did my own for the first time 🥹</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ewgrg3x7oj0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1gpwxmg</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>DIY Black Gel Nails</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4u5077venj0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1gpwxji</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>I did these 80s themed Max nails! 💙💚</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpwxji</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1gpwmtp</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Designed a set of press ons for a friend - brief was colour🌈</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9zxf575lj0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1gpwi5h</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Some press-ons i made!</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpwi5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1gpwgmi</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>new to me</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpwgmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1gpuv76</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Some nude nails this time! Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpuv76</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1gpwaom</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Some patterns</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5yj72lgij0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1gpw9rh</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press ons 🧚‍♀️ </t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpw9rh</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1gpw795</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t xml:space="preserve">November bday = November nails 🍁 🍂 </t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0gza0dsshj0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1gpw31n</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>burned brand new nails smoking - advice?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpw31n</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1gpvyow</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>A little red today.</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lcei10wxfj0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1gpvooz</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bright pink </t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9wzq3e0ej0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1gpu0c3</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>What is it about my nail shape that needs improving???</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpu0c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1gpuior</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>foil stickers really do the most sometimes ✨</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vywhr38i5j0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1gpt5hd</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>How do you clean up?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpt5hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1gpt1x4</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Nail broke, again.</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpt1x4/nail_broke_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1gpuent</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bridging the gap between autumn and Christmas - dark burgundy bows </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpuent</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1gpu1ce</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Doing my own gel. Please roast me! </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpu1ce</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1gpu0qu</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my sister's nails in honor of the upcoming Wicked movie 🪄 ✨ 🫧 </t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6axtnbs1j0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1gpt3se</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Should I stop BIAB?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpt3se/should_i_stop_biab/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1gpti7k</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Birthday set! I can’t stop looking at them ✨</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j1np1dozxi0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1gpthp4</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>New to press ons</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikvpcl2wxi0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1gpth0x</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel manicure i got today 💖 i feel so fancy with these </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpth0x</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1gpsto7</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Moo Deng nails 🦛</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yhndi13ti0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1gpspsq</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Disappointed with first gel set</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpspsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1gpsauk</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Beginner here, where to start?</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpsauk/beginner_here_where_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1gpry5h</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails by me </t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/47zp2gbqmi0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1gprx32</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>fresh set of metallic purple nails 🦄</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gprx32</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1gprp02</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>will my nail beds ever grow? i bit my nails for over 10 years, and have cut them short ever since. this is the longest they've ever been.</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1t6zf6vki0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1gpr0ax</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I think I finally got the hang of press ons! </t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpr0ax</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1gpqn8a</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made these press ons about 3 months ago now. (they look bulky because there’s tacky stuff holding them to my nail for the pics) they weren’t my fav but they also weren’t horrible </t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqad8p1ddi0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1gpqm9r</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fall florals </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpqm9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1gpqjix</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Banged up cuticles </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zb4yfn3mci0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1gpp905</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help me pick a signature style. </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpp905</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1gpq6dp</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>My Patriotic Nails</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bex2uoyu9i0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1gpp4em</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Newbie - help</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpp4em</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1gpp2aw</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>What nail shape would look best on my hands?</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t0019aes1i0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1gpoiuh</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t xml:space="preserve">another small update - using builder gel </t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpoiuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1gpoc2c</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hazy Autumn Vibes </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r22c1r4gwh0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1gpo4wm</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Colour opinion? </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpo4wm</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1gpnzb9</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>One of my favorites so far</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/51yg57rqth0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1gpnx3l</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Just a random nail day</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9iny9em9th0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1gpnmd0</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>protecting my nails from pottery?</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpnmd0/protecting_my_nails_from_pottery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1gpn7jc</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Switched to almond shape, new personality unlocked 🧸🍷</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7lk3n52unh0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1gpmxju</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone feel naked without long nails? </t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tel1wgnnlh0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1gpmq1c</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Nails I did for the Military Ball this year</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpmq1c</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1gpintn</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Opinions on the best nail shape and length for my fingers?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpintn</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1gpgv91</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn harvest gel nails. </t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyrpn162vf0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1gpm7sx</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>This gives me halo vibes 😇</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpm7sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1gpm2i5</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying tortoise shell </t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18qz8qgoeh0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1gplumn</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Tech did a terrible job, what should I do?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gplumn</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1gpluco</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Nails and manual labour</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpluco</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1gplfr9</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">private nail techs </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gplfr9/private_nail_techs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1gpkuy9</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween nails: Hand painted, no stencils! </t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1t7datr84h0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1gpkmfl</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Quite chuffed with my new set I painted last night. So much fun!👽🐄🧪</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpkmfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1gpjwvb</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did these on myself still need to manage the shape better </t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/055gbitjvg0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1gpj2p5</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on my nails? </t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpj2p5</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1gpik82</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Can nail products such as gel polish be harmful for the person painting the nails?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gpik82/can_nail_products_such_as_gel_polish_be_harmful/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1gpiaz6</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>I did them myself (first time)</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpiaz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1gpi3h9</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t xml:space="preserve">short nails :( </t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcf8n2ijbg0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1gq7yjw</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Pearly pink glitter gradient 💖</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t9uvj8sykm0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1gq703q</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Ilnp- Be Mine vs Mooncat- Your Hearts a Black Hole</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq703q</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1gq6rzp</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cannot express how much I love this polish </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq6rzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1gq5ldn</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Favorite “Orange Glow” Polish</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gq5ldn/favorite_orange_glow_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1gq5bbl</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Dupe for Tangee Red Coral (discontinued)?</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gq5bbl/dupe_for_tangee_red_coral_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1gq594e</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Playgirl 'Ios'</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/playgirl-ios-1oJvZEk</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1gq419m</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone recognize this brand of file? </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq419m</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1gq3sf2</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>such a farse by emily de molly!</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq3sf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1gq3nbr</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Lynn does these shimmery &amp; iridescent polishes so well! Here’s “The Plot Chickens”</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq3nbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1gq325i</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>IT’S HAPPENING!!!</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdt0krwy2l0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1gq2mit</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Colors by Llarowe Berries in the snow</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bp33unayyk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1gq2l5s</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Mooncat Cart Help!</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq2l5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1gq19kh</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>ILNP Hallucinate vs LynB Aquarius</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq19kh</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1gq11v1</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Polished for Days - Shadow on the Moon</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69mubtbykk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1gq053h</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>I Invoke Thee by Bee’s Knees Lacquer</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq053h</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1gpzul3</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>RIP broken nail</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1cnst1vak0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1gpzddm</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t xml:space="preserve">admiring my mani </t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4kqav7x6k0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1gpzazb</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>See Through You - Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpzazb</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1gpz90t</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has Essie Gel Setter turned yellow on anyone else? Brand new, unused bottle. </t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r64jjw6y5k0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1gpz63w</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Help. Is this second “nail line” bad/what is it/ how do I get rid of it?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nh0lo2m95k0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1gpz5x6</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Stronger Together</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpz5x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1gpyhq1</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>birthday manicure!</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpyhq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1gpxgix</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KB Shimmer “For The Pun Of It” </t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpxgix</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1gpxdih</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>a belated post for my already-belated spooky nails for a very spooky week 🌙🐈‍⬛👻</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpxdih</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1gpwwhj</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Unique orange shades?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpwwhj/unique_orange_shades/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1gpwuga</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>🧡🤍Stripey Socks🩵🩶</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpwuga</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1gpw7yk</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Me at my warehouse job &amp; not risking my nails to break 🤣</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4bf7u7uhj0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1gpvyhe</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Just letting everyone know…</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpvyhe/just_letting_everyone_know/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1gpvmn2</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Pregnant and freaking out about toluene!</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpvmn2/pregnant_and_freaking_out_about_toluene/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1gpv5iu</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Recs for grey polish with green shimmer?</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpv5iu/recs_for_grey_polish_with_green_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1gpulto</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Holo Taco: Playing With Sapphire</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6xjcjn56j0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1gpovnl</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Homemade cobalt glass jelly! (And learning more about how to make jelly lacquer look more like gel)</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpovnl</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1gptbai</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tortoiseshell nails are the ultimate autumn mani </t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gptbai</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1gpt4sz</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Joined in on the mourning mani’s, but with a ✨colorful twist✨</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpt4sz</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1gpt35w</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Look Alive! 🔮🪼</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpt35w</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1gpsok2</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Anyone have recs for a dupe of this F.U.N Lacquer magnetic gel polish?</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckhc05u1si0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1gpsnop</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Before the fire is out</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpsnop</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1gpsj0l</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Has anyone mixed nail polishes for desired color they couldn't find elsewhere?</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpsj0l/has_anyone_mixed_nail_polishes_for_desired_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1gprwan</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>This ILNP topper?!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vpnmtjjcmi0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1gprscv</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Is toluene in top coat really something to worry about for daily nail painters?</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gprscv/is_toluene_in_top_coat_really_something_to_worry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1gprke5</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>New nails for vacation!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ebvylqwji0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1gpqvmx</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>How do I love my nails?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpqvmx/how_do_i_love_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1gpqrrx</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>North</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpqrrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1gpqo26</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Accidentally gave myself a skin manicure</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpqo26</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1gpqmr2</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Something Witchy</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpqmr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1gpqlcg</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Holo Taco Brick Wall &amp; Scorched Earth</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c4ivmefzci0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1gpqa06</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Trying to cope with the last week with some shiny nails</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpqa06</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1gpq9uw</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Tried a new technique for my magnetic mani and it actually worked</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpq9uw</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1gppt62</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Nichibotsu</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5fkr5l087i0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1gppq3z</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>I can't get white polish to look non streaky and awful.</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gppq3z/i_cant_get_white_polish_to_look_non_streaky_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1gpp54p</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A set I did a while ago 🌟🫧 </t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpp54p</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1gpotsr</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Caramel Apple vibes 🍎🍮✨</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpotsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1gpnxtm</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Destashing feels as good as adding </t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpnxtm/destashing_feels_as_good_as_adding/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1gpmoku</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Ballet shoe French mani</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6496lzojh0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1gpm5dr</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP has a new customer </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpm5dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1gpllgz</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What is the new holy grail quick dry top coat? </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpllgz/what_is_the_new_holy_grail_quick_dry_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1gpld83</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Nail Health Supplements?</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpld83/nail_health_supplements/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1gpkxnx</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Eye catching 💜💚💛🩷</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpkxnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1gpkpxl</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Dam nail polish - AHHHH!</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpkpxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1gpkmzo</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>ILNP Petals 🌸</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/letl9qrb2h0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1gotalr</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Name that color!</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gotalr</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1gp87qq</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Can't get gel nails off 😩</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g50foophad0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1gpjjbr</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Eternal glow indeed ✨</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpjjbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1gpidp6</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Belated Diwali Nails!</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpidp6</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1gphb47</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Is this gel-like base coat harmful?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjcowz531g0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1gpgyse</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>I can't seem to stay away from the cuticle ☹️</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gpgyse/i_cant_seem_to_stay_away_from_the_cuticle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1gq4wt9</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Painting a Jinx Nail set and this is me 5 hours in 🫠🥲</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m8zuayvkl0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1gq4a8m</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Olive martini nails 🍸 </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xc57r5mjel0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1gq3yj7</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>WWYD?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjentnzabl0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1gq3hcd</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>A set of nails i did recently inspired by the 2010’s internet</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q2sfcm8r6l0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1gq3dmd</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>BlindedNailTech</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq3dmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1gq37xo</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Love this design</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq37xo</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1gq1azm</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Amé este diseño 🖤</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rxffn56nk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1gq1925</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Holiday starry sky 🌌</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nnxfhvomk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1gq0m27</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>new to nail art, proud of this set 💖</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gel16cm7hk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1gq04ym</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>New set ❤️‍🔥 would you do them?</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fa3nm67dk0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1gpys80</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Miffy/Nijntje</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpys80</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1gpxcne</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Concept vs Outcome</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpxcne</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1gpwuh6</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>some press-ons I made recently :D !</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpwuh6</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1gpw2xe</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Is it Fall Season Already🧡🤎</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/691334kxgj0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1gpsvzk</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>I love blue nails</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5w2qlckti0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1gprcde</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Cats Eye</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hu7frrkbii0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1gpr1lm</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite Nail Tools/Techniques? </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gpr1lm/favorite_nail_toolstechniques/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1gpqo1o</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Fall florals</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpqo1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1gpoba5</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Taking advantage of watering day 🪴to show off my snowy pink ombré </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/160aoneawh0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1gpo254</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What would you call this set? </t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpo254</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1gpn9ay</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>I feel like this color looks great on me🥰 what do you think?</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w3zthb38oh0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1gpmdad</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Soft gel extensions first trial </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2m12476hh0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1gpl83x</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Sweater nailsss</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpl83x</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1gpkfu4</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mis lindas uñas </t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gpkfu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1gphq35</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>First Try with Nail Art! Went for an OG DBZ Theme</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gphq35</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1gpg9ia</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dreamy chrome obsession </t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q7ka00cimf0e1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Nov 14 08:11:00 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_17.xlsx
+++ b/data/collected_data/2024_11_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C681"/>
+  <dimension ref="A1:C842"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12011,6 +12011,2743 @@
         </is>
       </c>
     </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1gqzsd6</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got the cutest set done today! </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0ky0wxpnt0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1gqyzf8</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish never dries </t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxdodnq3dt0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1gqxoaj</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How bad is quick fry for your nails, really? </t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0oly91sxs0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1gqx7gf</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>DND LED Lamp V3 - Question</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqx7gf/dnd_led_lamp_v3_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1gqwxjz</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Need some tips on how to use this tool properly!</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4skg2w7zps0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1gqy4u5</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Natural press ons!</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o2hijgzr2t0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1gqy2pl</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>These were my nails last time but I wanna get something similar again</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmj8vw352t0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1gqxt5y</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Obsessed w cat eye right now</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxy9c62azs0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1gqvfw3</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>HELP… PLEASE… 😅</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgilgu29bs0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1gqvw66</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just got my claws painted </t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6h7o9mpkfs0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1gquqk1</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Shape help - Rainbow Nailbed</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n90yuzgp4s0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1gqv06m</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I want polish that peels off easily</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqv06m/i_want_polish_that_peels_off_easily/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1gqvrt3</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Why can’t I get a smooth top?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x6yun4gees0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1gqvnji</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t xml:space="preserve">thermal moody purple nails </t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co9ckrn9ds0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1gqvl4c</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>fall nails that match my brindle baby 🥹</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqvl4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1gqvj49</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Topaz nails for November</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqvj49</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1gqvi29</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Shard 💜</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqvi29</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1gqvcxj</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>On a journey</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uc50g7thas0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1gqv0vq</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>did some clear nails this week! 🩷</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqv0vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1gquz9x</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Soft pink/nude set 😊</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwl6c6kx6s0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1gquwk3</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/joapz5b86s0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1gqrzew</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter set </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7ufljgdgr0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1gqszki</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Halloween Nails Pt.2 </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqszki</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1gqsnpe</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>How much do you tip your nail tech?!</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqsnpe/how_much_do_you_tip_your_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1gqsl90</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>How do these look?</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqsl90</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1gqs7tw</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>my nails 🖤</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkoth8ibir0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1gqs2q8</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>I always ask for tortoise shell in November! So classy and it’s a set I get the most compliments on</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tkmyqd15hr0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1gqrxae</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Summer in the Fall Nails</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqrxae</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1gqrwzr</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Finished painting one of the jinx nails! 2 days later 😫🫣</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awkypogsfr0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1gqrjo9</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>How long do your nails last</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqrjo9/how_long_do_your_nails_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1gqqcpn</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday set! </t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2p7su0xz2r0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1gqpl30</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>What do you think about this design?</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sf7ebgtywq0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1gqp94b</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying the cat eye + jelly polish trend </t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqp94b</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1gqog4z</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanted to share the lovely bday set I got 🥰 felt like an ice queen </t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8eakg94oq0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1gqoakq</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails </t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqoakq/press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1gqo8tp</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>I got a soft gel manicure for the first time. I'm really impressed!</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez64723kmq0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1gqo5vn</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So proud of my fall nails! I can’t stop looking at them! </t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fk3qyczlq0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1gqnwf0</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Gel mani on my natural nails</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqnwf0</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1gqnczd</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Classic red cateye ❤️🖤🥲</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2v0wha0zfq0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1gqmfi5</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Emerald nails 💚🌲🧙🏾‍♀️</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0u2y20r19q0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1gqmcbr</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zetwcfzd8q0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1gqmaqq</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time I do french manicure to myself. What do you think? </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mg83g128q0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1gqlf4f</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Had a cut on hand, getting nails done later (gel manicure); will there be any issues?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqlf4f/had_a_cut_on_hand_getting_nails_done_later_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1gqlu0y</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>I got my nails done last week and I'm not happy with then</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqlu0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1gqm205</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>aurora jelly beans</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqm205</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1gqly1n</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>pink french tips 🩷🌸</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qqp6yumb5q0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1gqljge</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy Coincidence </t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqljge</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1gqlbt3</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Gel X at home</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqlbt3/gel_x_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1gql2qk</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Tried doing a new shape on myself, what do ya'll think?</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gql2qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1gql0g0</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>I love this color!</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mle0l2kcyp0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1gqkp2r</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Smashed fingernail - might get ripped off</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqkp2r/smashed_fingernail_might_get_ripped_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1gqkmyn</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>I got the contact dermititis &lt;/3</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqkmyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1gqkr2w</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will attack if provoked </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2ymgwrgwp0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1gqk967</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>I did my sister's beautiful nails:D What do we think?</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/627faw5vsp0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1gqk8lw</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set! Sun and moon for my anniversary 💕 </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqk8lw</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1gqj5q4</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">at home manicures </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqj5q4/at_home_manicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1gqa4rf</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>What should I get?! Helpppp</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqa4rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1gq7e6l</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Be honest…how bad are they? </t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq7e6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1gqdx1b</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know what is this and how to get rid of it? </t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un1cyw51ho0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1gq80o2</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Business casual nails?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gq80o2/business_casual_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1gq7byw</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>My sailor moon inspired nail art 😭🌙💕</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7g95nkmcm0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1gqi9c8</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Galaxy 🌠</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqi9c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1gqhowa</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>They look pretty</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tk4r7yt4ap0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1gqgt3s</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Press-ons with acrylic paint</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqgt3s/pressons_with_acrylic_paint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1gqhcnj</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Haven't done my nails in ages due to excessive shaking, so this feels amazing</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4h2743n7p0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1gqh70s</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Does this suit me?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5dydd0g6p0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1gqgvpk</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🩶 </t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqgvpk</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1gqgjcw</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails from last month </t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqgjcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1gqgggn</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Gift Ideas for Young Nail Enthusiast?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gqgggn/gift_ideas_for_young_nail_enthusiast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1gqga8z</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>DIY Fill: Morovan Solid Nonstick Solid Gel</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqga8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1gqfzkk</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wavy Gel Manicure??? </t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqfzkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1gqfy0o</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>I made some claws on myself today 🐱</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqfy0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1gqflup</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Like the length, the color and shape. What do you think?????</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jo254lhluo0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1gqfkls</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Gel on natural nails. Loving this design, what do you think?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbnv22vbuo0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1gqf1hv</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So happy with this manicure </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqf1hv</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1gqek3w</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Orangy and gold witchy girly-pop nails 🍂</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqek3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1gqdd9d</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Natural nails since yesterday</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gueurl6bco0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1gqd95e</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>El rojo siempre ❤️</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pm2ix07abo0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1gqd0mq</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>got my nails done today!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oykpgb619o0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1gqbl4f</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Some halloween nails I did this year - what do you think? 💕</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7127b2mgvn0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1gqbig9</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>My nail extensions keep falling off</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rk5n3joun0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1gqaw5m</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got these done yesterday </t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ay4kfzwpnn0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1gqa7w3</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Did these on my friend✨💅🏻</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v1pnnl9ofn0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1gqxw2c</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Manicures of the last couple of months!</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqxw2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1gqx6w3</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is Queen of the Dead by mooncat a shimmer? </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zw4vupross0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1gqvgxz</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I need emotional support :(</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqvgxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1gqvgw9</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Shard 💜</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqvgw9</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1gqup0v</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>thermal purple+glitter！</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqup0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1gquhl6</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I DID IT!! </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gquhl6</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1gqu6vm</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Today's nails</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqu6vm</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1gqtsuq</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>It really is wild</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/afhirtv3wr0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1gqtcoa</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Best nail polish rewards programs?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqtcoa/best_nail_polish_rewards_programs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1gqtcfu</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Finally love my nails :,)</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqtcfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1gqtags</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>i've been working on nail shaping lately, and i think i'm making good progress!</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipscn6smrr0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1gqt6p8</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any regular polish dupes for this gel? </t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqt6p8</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1gqt58m</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Essie Shade not available in Canada?</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqt58m/essie_shade_not_available_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1gqsmrz</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was it good? </t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oahik8vlr0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1gqsgjj</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Sweater nails 💅🏻</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqsgjj</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1gqsdn4</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Sparkly blue</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqsdn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1gqs1tr</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Cirque Colors: how do you achieve this style?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqs1tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1gqrl4y</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>trying this natural nail thing again…</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xa456s42dr0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1gqqqff</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>ILNP Rosalie</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n87uu2a06r0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1gqqg3e</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>I wanna try some nail polish what is a good brand with like a kit on Amazon?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqqg3e/i_wanna_try_some_nail_polish_what_is_a_good_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1gqovkr</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>How are y'all keeping track of your Black Friday wishlists?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqovkr/how_are_yall_keeping_track_of_your_black_friday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1gqoj2n</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Prism Polish Multichrome makers -worth it?</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqoj2n/prism_polish_multichrome_makers_worth_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1gqoc40</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>new job as a magical forest spirit</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmjknvz9nq0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1gqnts2</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>A set I did while waiting for my short rib soup to tenderize!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqnts2</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1gqnokq</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Merkitten is the pink of my dreams</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqnokq</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1gqmxqa</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>yucky cat claws</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rcw6qascq0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1gqmx2d</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Fall Nails 🍁🍂</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dfsegfrncq0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1gqmo6u</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Light My Fire + Pyro</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zrkuumguaq0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1gqm3si</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>aurora jelly beans</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqm3si</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1gqlhz2</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>CHOOSE MY NEXT MANI!</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1wm7b612q0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1gqlcz0</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>What are everyone's Black Friday plans?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqlcz0/what_are_everyones_black_friday_plans/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1gql1qx</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Freshly Bitten vs Cockadoodle Doom? </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gql1qx/freshly_bitten_vs_cockadoodle_doom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1gqks0s</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maybe a little too picnicy for the weather but I couldn’t resist </t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwn3ji0owp0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1gqkgfb</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inadvertently created a fun combo trying out my new polishes </t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw1ewx7dup0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1gqjzv2</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>why did this happen?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqjzv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1gqjvw4</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Mooncat’s Illusionist 🔮</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gd1nwjp3qp0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1gqjveg</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Nails are a mess after nail varnish removal?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqdqjdc1qp0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1gqjv4h</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>This is my own private domicile and I will not be harassed!</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6mxceyypp0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1gqjsb9</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Church, The Cat 🐈‍⬛</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqjsb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1gqjnd1</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Glowy shimmer + holo 💙</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqjnd1</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1gqjeiz</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first Holo Taco!!! </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqjeiz</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1gqjcdh</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Any recommendations on how to achieve this shimmery nude/cateye-esque with Lacquer?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k3u0fm0ulp0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1gqjbst</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Black Friday?</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqjbst/black_friday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1gqixz8</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>🍁Fall Leaves🍁</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqixz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1gqiw7q</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Anyone have experience with Don Deeva?</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqiw7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1gqi1ob</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will attack if provoked </t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqi1ob</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1gqhpdk</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A Rose Amongst the Weeds </t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgbw7dc8ap0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1gqgyha</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Ethereal Hecate</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqgyha</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1gqgbgh</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>A leetle beetle of colour to the dark, murky late autumn</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b83onuizzo0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1gqgabp</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape suits me better? </t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqgabp</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1gqfwfg</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best light blue metallic </t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqfwfg/best_light_blue_metallic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1gqfnim</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Birthday celebration nails</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pilkxvbyuo0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1gqfg2b</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Im so proud of these🥹🥹🥹</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqfg2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1gqff1d</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Prism Polish - Walking on the Sky</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8kf8hia5to0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1gqf0fq</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Flashing Lights ILNP</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q9el3rezpo0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1gqesn8</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Nail decal question! How do I find the flat decals where you slightly wet a piece of paper, and they slide off like temp tattoos? Do they have a name?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqesn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1gqeexu</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>So shifty</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vj43xdf8lo0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1gqdigo</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Learning I am having an allergic reacting to Gel-X, can I do press ons? </t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqdigo/learning_i_am_having_an_allergic_reacting_to_gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1gqdhpw</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Similar polish to Julep Tanith?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqdhpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1gqcoa5</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cozy Fall Mani - OPI Cliffside Karaoke </t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqcoa5</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1gq21r4</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>DIY Mauvey "Started-As-a-Jewel-But-I-Think-It's-Now-a-Geode" Set</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq21r4</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1gq2zi4</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Eye color nail polish</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zn57785a2l0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1gq6zc4</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Struggling with Cat Eye Gel Polish - Need Tips!</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gq6zc4/struggling_with_cat_eye_gel_polish_need_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1gq9r4c</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Very demure, very mindful</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6tsrqtl9n0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1gq874r</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>A shifty dream</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gq874r</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1gqyqm9</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Gold recommendations??</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqyqm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1gqry3u</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter set </t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ivqrbh2gr0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1gqrwjn</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Finished painting one of the jinx nails! 2 days later 😫🫣</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqrwjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1gqru1p</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Glazed ✨</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqru1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1gqrmtb</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Super Duper pigmented liner gels like pots- but  Preferably in bottles.</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8t4d7hfdr0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1gqm7ol</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>aurora jelly beans</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqm7ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1gqktry</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t xml:space="preserve">third set I ever made lel </t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqktry</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1gqkmgh</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>I love when I draw 🥰</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko9xh6zjvp0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1gqj52i</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>I do really like these ones 😩</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iuaf66smkp0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1gqiokq</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Which design do you prefer?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqiokq</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1gqgni7</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Holiday Nails ❄️ Snowy Night</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqgni7</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1gqfuin</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Gaudy Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z441xhnfwo0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1gqbki3</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Some halloween nails I did this year - what do you think?💕</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqoxt1p9vn0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Nov 15 08:10:52 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_17.xlsx
+++ b/data/collected_data/2024_11_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C842"/>
+  <dimension ref="A1:C1022"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14748,6 +14748,3066 @@
         </is>
       </c>
     </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1grq6m4</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>How to take off press ons if I want to reuse them?</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ui8spl1be01e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1grqz8f</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Need Stiletto and Square XXL inspiration</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grqz8f/need_stiletto_and_square_xxl_inspiration/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1grr5wn</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>I Like it, but im not happy</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grr5wn</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1grr2fn</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Do u guys think this looks cute?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9t8y3ajp01e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1grptig</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>For the Pun of it (KBS) vs Jewel Beetle (MC)</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grptig/for_the_pun_of_it_kbs_vs_jewel_beetle_mc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1grpmy7</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Topaz Tears</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/izytcibv701e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1grp2xj</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>I can’t find the original posters post, I scrolled and scrolled and scrolled, but couldn’t find it :(</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pewgmcir101e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1groyo3</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Male here first time posting </t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u57r5j8j001e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1grotuz</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>a nail biter just trying out nail art</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grotuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1groqgf</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Favorite gel sets from this year! ⭐️</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1groqgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1grnioj</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Marble </t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grnioj</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1grlj17</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>This is so annoying</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozxfk0xs2z0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1grllnc</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Soul eater inspired nails</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grllnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1grjkn1</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are some good liquid nail glues? </t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzlhjqo7ly0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1griz0t</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Russian manicure didn’t cure all the way </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1griz0t</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1gro10n</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Love the purple and pink</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxsyn6puqz0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1grnxht</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>went super short for the first time!!</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sd2rnfqwpz0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1grnsv2</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Acrylic fill already separating and breaking after six days</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grnsv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1grnhs5</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my nail lady </t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grnhs5</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1grnc8m</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Color match gel polish for Mia secret cover pink acrylic </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grnc8m/color_match_gel_polish_for_mia_secret_cover_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1grn9gv</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own nails. Not perfect and a little long for my liking but getting used to them. The color is china glaze black diamond. </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8ymjn95jz0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1grn7mh</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grn7mh</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1grn4jz</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Short nails, but discovering wraps has helped them grow</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x6c5vduhz0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1grmyhz</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Short nails 🙃</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grmyhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1grmrqa</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Would Like to Start Painting with Eyeshadow </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grmrqa/would_like_to_start_painting_with_eyeshadow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1grm2oy</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Set I’m working on atm…</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87d1nrct7z0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1grlsfm</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Give me your tips for jelly polishes! </t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grlsfm/give_me_your_tips_for_jelly_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1grlq3e</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>My first gel x set I did myself - tortoise shell 🐢</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grlq3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1grl76v</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>I need some advice</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7l29j7qzy0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1grk7lh</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Rare 😍 sometimes its hard to click on my phone 😁</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko9wn65tqy0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1grk1xa</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>New to doing my own nails, I'm obsessed with the glitter 😍</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8ijq6nfpy0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1grji95</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Opalescent nails @isabelfreitasnails</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4gmmjojmky0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1grj5c3</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>the wrong nail broke (arcane)</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhf508kmhy0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1grj1y1</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>💓</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dz03l6vgy0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1griu5i</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Apparently I'll always be a press on kind of girl 💅🏻</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r0565lvzey0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1grimzw</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>What do you use for strong nails?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grimzw/what_do_you_use_for_strong_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1grijrq</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Under nails after refill? </t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqayhjujcy0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1gri1k2</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Super pigmented gel paint - preferably in bottles </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gri1k2/super_pigmented_gel_paint_preferably_in_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1grhoao</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Told my nail tech to do whatever she felt like</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grhoao</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1grga7j</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had acrylics removed and this is how my nails look after. Is this normal or did they completely eff up my nails? </t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grga7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1grguvj</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>I did my friend’s nails ☺️</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h1awfpsyx0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1grgus4</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>First DIY of lockdown 2020 to 2024 BIAB DIY</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5t7vdctryx0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1grg9q1</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>I feel like there are a lot of colors but what do you think?</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/609g7ba8ux0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1grfi2i</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>First ever manicure. Nailed the inspo</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grfi2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1grdyhg</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>How can I stop this?</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xv8sza5bcx0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1grf8fz</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>are we obsessed or obsessed?</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wf7s81r4mx0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1gre30z</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Christmas Nails🎅</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gre30z</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1grdiqf</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Been into shorter nails lately and I love these</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ychez0qz8x0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1grdi0v</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>First time doing nail art, how did I do?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grdi0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1grdgcf</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>New to making my own nails.</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j6ada1bg8x0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1grcr2h</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Does this look as ridiculous as it feels?</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfljte763x0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1grd9un</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>tips on structure manis + nail art</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grd9un</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1grcu3s</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Help removing remnants of gel</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqy27vrs3x0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1grcsuh</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I let my gf “practice” on my nails, and she did so good! </t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grcsuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1grclb1</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Suggestions for Weak Nails</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grclb1/suggestions_for_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1grcjud</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome nails </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fsst9uin1x0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1grc0l3</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>How do I get better at painting near my cuticle?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmufc7emxw0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1grcmrh</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Nail Strengtheners</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grcmrh/nail_strengtheners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1grcl3d</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Latest Set 💅</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bwass3iw1x0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1grc8g9</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Did a Jigglypuff set for an upcoming SSBM tournament!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grc8g9</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1grbu4l</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel advice? </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grbu4l/builder_gel_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1grc0yh</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>I did my nails with gel polish for the first time!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grc0yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1grbeho</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>What nail shape suits me?</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gt0hklrysw0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1grb0oe</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>NyQuil Nails</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grb0oe/nyquil_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1grb070</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Practising building proper nail structure and shape while going out of my shiny and sparkly comfort zone. Any tips, how to not make them bulky with colour and top coat?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grb070</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1gray18</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Been getting this gorgeous beet root color done for this season 🥰</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gray18</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1graisn</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Fresh</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rv4kekrhmw0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1gragkn</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Loving winter tones finally!</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gragkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1grabgv</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>What can I do better? Second time trying to do at home.</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grabgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1gra7iv</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Press-ons on ski slope/jump nails</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gra7iv/pressons_on_ski_slopejump_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1gr9r61</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>'Former' nail biter reporting for duty!</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr9r61</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1gr9nx2</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Non toxic alternatives?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gr9nx2/non_toxic_alternatives/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1gr9npa</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2nd time DIY gel, chose Cow print! </t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kp1ylv0gw0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1gr88br</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Christmas nails I did</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr88br</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1gr83cl</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Male here, expanding my comfort zone 🙂</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr83cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1gr7oui</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Client wanted Korean/Chinese Inspired Pearl nails 🤌✨</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to8pkli41w0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1gr7agx</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr7agx</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1gr6t5k</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Can this be fixed through soak off or fill? Don't think it's broken all the way through</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yryt5p8uv0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1gqyqa8</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Nail growth after being a biter for 10+ years</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/057ij68t9t0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1gr0syn</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>going on hour 8 for these press ons im making! pinkie pie nails 🍰 loosely inspired by joh.nail on IG :)</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr0syn</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1gr6a1v</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Biab on natural nails, what do you think of the designs?</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh34oq00qv0e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1gr5a4w</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>1st time to wear this nail extension. is it pretty?</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dcbrrpxihv0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1gr4ihs</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat Eye? </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gr4ihs/cat_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1gr4hsh</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Simple Christmas Nails 🤍❄️</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5axaeaicav0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1gr4gv6</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Not one to do my nails but here we are</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr4gv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1gr49v9</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Seashell nails 🐚</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cy1egzo78v0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1gr3pvi</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Nails at home!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr3pvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1gr3blg</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Classic red🍒</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3h3x82ceyu0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1gr3469</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>What is wrong with this profile ? It is a mid length almond shape but the side profile looks off</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vme2ebq5wu0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1gr1jfd</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Small air bubble on gel on natural nail - dangerous???</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mhki2e6cu0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1gr19ud</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Slightly messy application but iridescent nails are beautiful </t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr19ud</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1gr190z</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Ghost Pokemon nails </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr190z</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1gr13dv</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>What can I do to keep my nails from breaking?</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gr13dv/what_can_i_do_to_keep_my_nails_from_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1gr0qpu</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Fuchsia 🐙🎀</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vswqk0531u0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1grqdra</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>My heart…</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hi1uwwpqg01e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1grpybg</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>You were raised in the prug…I was born in it 😷</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grpybg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1grpnqr</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>ILNP Cityscape is so beautiful!</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/94r2wl29801e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1grples</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>jelly gel polish not adhering and curing properly, help!</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grples/jelly_gel_polish_not_adhering_and_curing_properly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1grpc4c</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Really needed something bright 💖</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grpc4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1grokgv</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Tell me about peeling basecoats!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grokgv/tell_me_about_peeling_basecoats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1grn6ao</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Atomic Black Friday Sale?</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grn6ao/atomic_black_friday_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1grn3fz</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Hunt for the perfect rose color</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cv4lanjhz0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1grllrx</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Poisonberry &amp; Pomegranate Seeds from Mooncat 💟💜💅</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grllrx</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1grljs3</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Two versions of the same mani</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grljs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1grlc32</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Nails Inc having same packaging as Butter London?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grlc32/nails_inc_having_same_packaging_as_butter_london/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1grl41y</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Trying to find gel polish in one of these colours</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grl41y</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1grky95</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it just a bad match for me or is Grace-full nail polish generally not very good? </t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grky95/is_it_just_a_bad_match_for_me_or_is_gracefull/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1grkq28</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Brick pattern nail stamp</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grkq28/brick_pattern_nail_stamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1grknf9</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>I’m 10000% sold on nail “concealer”</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0b3xe9apuy0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1grka6l</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Rainbow topper</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grka6l/rainbow_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1grj2ry</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Does anyone have Happy Haunts or Come Out to Socialize PFD and River Styx Mooncat?</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grj2ry/does_anyone_have_happy_haunts_or_come_out_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1grio3b</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Power Color Thursday</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grio3b/power_color_thursday/</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1grhi3x</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Batgirl and Witchcraft from Pahlish</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grhi3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1grhhf8</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Do You Try To Limit Your Collection Size?</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grhhf8/do_you_try_to_limit_your_collection_size/</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1grgzl9</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP — chocolate slate </t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grgzl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1grgpf9</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>Polishes Used: LynBDesigns (Shade: Heroes Come In All Sizes) | Seche Vite (Shade: Gel Effect Top Coat)</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grgpf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1grgf2s</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>fall beige mani 🤎</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grgf2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1grg701</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>The Artist</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grg701</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1grg6j4</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>How to destash polishes with bad formulas?</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grg6j4/how_to_destash_polishes_with_bad_formulas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1grfimd</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You all have sufficiently convinced me. Presenting: my first ILNP Order </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grfimd</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1grf728</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Phoenix Indie - Bill</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/42tptpjulx0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1gre8ez</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Ridge filler recommendations</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gre8ez/ridge_filler_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1grdicn</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Got a freebie today!</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u79so0uw8x0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1grdhdi</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>CHOCOLAAAATE!!!</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grdhdi</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1grd6ed</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Swatch request: ILNP “Midnight Kiss” and OPI “Chopstix and Stones”</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grd6ed/swatch_request_ilnp_midnight_kiss_and_opi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1grd5a7</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>recreated a sold-out favorite?</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grd5a7</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1grcrgv</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Sticky/bonder base most similar to Orly Bonder Base, just *without* being tinted orange?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grcrgv/stickybonder_base_most_similar_to_orly_bonder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1grci0u</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Dupe for cracked every cloud has a pink lining</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grci0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1grc445</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>my attempt at recreating a polish</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grc445</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1grbr92</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>mooncat’s “Blood Moon”🌙🖤✨🔮</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rd2428rmvw0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1grbqhs</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>✨ Phoenix Indie Polish, The Mirror ✨</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grbqhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1grb64f</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Shopping from my collection because I have a problem</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p7zdxwx7rw0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1grb5rt</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Looking for dupe- China Glaze Hunger Games collection cir. 2012- Mahogany Magic</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grb5rt</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1gra9ra</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Pinky purples are still seasonally appropriate, right?</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gra9ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1gr9tos</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seche Vite ruined my perfect manicure </t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr9tos</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1gr9set</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Blooming Azalea😍</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr9set</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1gr9rjy</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My attempt at the cat eye nail. </t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5w08jowgw0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1gr9hn9</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yes, OPI Nail Envy works. </t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dq3rulvew0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1gr95u7</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>🌈🖤 A literal (dark) rainbow on my nails</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zugydcbobw0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1gr8wu5</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Can it be saved with thinner?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mivmiudeaw0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1gr8uj5</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Where Am I?</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr8uj5</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1gr8nca</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Starrily's King Midas is back in stock!</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr8nca</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1gr8h28</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Is ORLY rubberized bonder hard on anyone else's nails?</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8nf1enu07w0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1gr83gy</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Can anyone ID this purple jelly?</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gr83gy/can_anyone_id_this_purple_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1gr80h5</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newbie attempt! </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sjc6edll3w0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1gr7x71</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Sparkly shifty green</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr7x71</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1gr7jxd</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t xml:space="preserve">holiday manis are in!! </t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rlxms230w0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1gr7iks</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Warm Dark Reds </t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr7iks</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1gr7bf5</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Dragon Scales vs. ILNP multichrome flakies - dupe or no? </t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gr7bf5/mooncat_dragon_scales_vs_ilnp_multichrome_flakies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1gr79zc</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>So shifty</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fusaodfvxv0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1gqv4pt</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Tips for Long-Lasting Gel Manicures at Home?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gqv4pt/tips_for_longlasting_gel_manicures_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1gqvs30</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Good GLITTER polishes?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gqvs30</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1gr6ncf</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best linear holographic with a nice base color? </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gr6ncf/best_linear_holographic_with_a_nice_base_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1gr6mth</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new favourite color! Three times three </t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr6mth</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1gr61ux</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Written Invitation is so pretty under the moonlight 🌝</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ms35f04vnv0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1gr5zrj</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Penelope Luz Divine Sky 💙💙</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr5zrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1gr5zqb</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Verdigris</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr5zqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1gr5ejl</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>DVN Black Friday sale? (And swatch request)</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gr5ejl/dvn_black_friday_sale_and_swatch_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1gr501j</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clionadh Cosmetics - Waltz of the flowers </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr501j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1gr4ytr</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>✨✨✨</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr4ytr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1gr4wvz</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Best topcoat to make holographic polish stand out?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gr4wvz/best_topcoat_to_make_holographic_polish_stand_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1gr4ivn</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Ether Dragon is just so mesmerising 😍</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr4ivn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1gr4hvf</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>How to achieve this effect?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nk3jk60dav0e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1gr3dyt</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Falsies keep popping off</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gr3dyt/falsies_keep_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1gr3d36</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>You Shall Not Pass! (but you shall shift)</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr3d36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1gr0wt9</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Autumn nails 🍂 </t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr0wt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1grr7r0</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Celebs sticker art !</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p2p18hvir01e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1grqnta</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>2nd DIY Press On Set</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grqnta</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1grqcxv</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>DIY nails</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grqcxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1gro2oq</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love the Pink and Purple </t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3wqnnkbrz0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1grm3s2</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Set in progress what do we think?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz0hcyw38z0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1gri3ur</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pigmented art gel paint question </t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gri3ur/pigmented_art_gel_paint_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1gra6wg</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newest nail dump! </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gra6wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1gr9m26</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I loved it 🥰 </t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0pfed7rfw0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1gr7znu</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Plaid transition nails</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1haqvk0g3w0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1gr78mf</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is the underside always this pretty </t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bd4rpefoxv0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1gr6tsq</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>First Christmas set EVER</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr6tsq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1gr5oqi</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Holiday-ish nail season starting 🌟</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr5oqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1gr4h8s</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Simple Christmas Nails 🤍❄️</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rvugax6av0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1gr4121</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Did some witchy nails!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gr4121</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Nov 16 08:09:48 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_17.xlsx
+++ b/data/collected_data/2024_11_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1022"/>
+  <dimension ref="A1:C1198"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17808,6 +17808,2998 @@
         </is>
       </c>
     </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1gshj9b</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes, air-dry top coat is better, I think. </t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gshj9b/sometimes_airdry_top_coat_is_better_i_think/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1gsg5ix</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>which shape looks best on me?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsg5ix</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1gsfda2</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspo pic by @isabelmaynails on Insta via Pinterest </t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezy60hhjx61e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1gsfgdm</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Press ons have come a long way.</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsfgdm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1gsfc83</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do y’all think </t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5o2wqe7x61e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1gseole</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving the BTartbox nails </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gseole</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1gsekhk</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Freshly made manicure 🥴😭</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uyiykp01p61e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1gsejgc</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>🐳</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7junroqo61e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1gsegj0</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Gel nails bubbling</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsegj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1gseafl</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>new nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uldkc7kam61e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1gse9d4</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Auburn nails for the fall! ♥️</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dc6emwwyl61e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1gsdxa0</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Obsessed with my nails 😍</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9ujz0puli61e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1gsdw47</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my BTArtbox nails but idk how to prevent bubbles </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsdw47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1gsdvqg</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Sizes for selling pre-made press-ons</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gsdvqg/sizes_for_selling_premade_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1gsdu5k</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Taste the rainbow 🌈</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/courageousterriblelorikeet</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1gsd6jz</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>This is my first time using press-on nails, how long do they last?</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsd6jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1gsd5u3</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Blue celestial cat eye 😍</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vz8zcmira61e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1gsckds</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Wrong color! What to do??</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsckds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1gscnii</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Look at this cute set!</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asc2d8v3661e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1gscsqv</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>October Nails</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkf6h1ug761e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1gsclnp</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>When your nails match your coffee :)</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxvqc7nl561e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1gsce38</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Every time I’m about to do something new, I take time to admire how far my nails have come! 🥹</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsce38</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1gsbkro</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Obsessed with the glass type look</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lj5941tv51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1gsaz8u</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Day 3 of doing my nails at home</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsaz8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1gs9kf6</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Two coats of funny bunny and one coat of bubble bath on top 🤍🫧</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c3g61vb8e51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1gs9hia</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Can I use Gelish base/top coat with OPI Gel color?</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/no72lwbkd51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1gs8z55</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Black matte gel nails </t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epe7c8qc951e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1gs9cmf</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Fall nails</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrslfrwfc51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1gs8bf4</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Want to remove glue without damaging my acrylic nail.</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipd3hvjy351e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1gs8ipy</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>New set for the holidays✨</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6e7ypwsl551e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1gs8gfo</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Eras tour ready 💅 </t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e1okp643551e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1gs7fmh</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>How necessary are dehydrator and bonder?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gs7fmh/how_necessary_are_dehydrator_and_bonder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1gs74e2</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Which Nail Shape Do You Like Better? Left or Right</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cljk7kdlu41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1gs72gv</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love different length and shape on my hands 😄 </t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5h4ijn5u41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1gs6wfk</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Trying out spinning charms</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/youdywnss41e1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1gs6vmz</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>New nails, what do you think? 🌺🩷</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs6vmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1gs6svm</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Orly Light My (Camp)fire </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs6svm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1gs6p6a</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Fresh and sharp</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs6p6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1gs6by9</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time getting a red manicure </t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs6by9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1gs671o</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>I love doing mixed media nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs671o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1gs5y6k</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>I'm not sure if I like them or if they're boring 🫠</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mj3yat93l41e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1gs5mav</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Looking for shades that could fit a Jinx manicure !</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzzt27yhi41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1gs5dgl</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>New nails ✨</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss6nbhpmg41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1gs53kc</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>How do I fix this? 😭</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jiibc7tie41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1gs3rg9</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>recommendations for primer &amp; top coat?</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gs3rg9/recommendations_for_primer_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1gs3yqj</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>After four years training in Russian shops I’m finally good enough for the close ups</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/paq5rvdq541e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1gs4ndr</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice? </t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs4ndr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1gs4xaf</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Go easy on me! </t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gs4xaf/go_easy_on_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1gs4rf5</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>my simple nails</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onf97zwwb41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1gs4r6m</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>They’re fire</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s68i2t6vb41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1gs440h</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>My nail tech NEVER disappoints 😍</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs440h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1gs40x0</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Having problems with gel manicures lasting! Recommendations?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gs40x0/having_problems_with_gel_manicures_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1gs3z0k</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>4th try!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs3z0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1gs3ti5</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>What could I have changed to make them less “boring”</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4i1ed8q441e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1gs3p4q</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Do you like them?</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vz31qvss341e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1gs3iot</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Male Looking for Fresh Nail Design Ideas – Here's My Last Sets.</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs3iot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1gs25j3</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>hii, feeling comfortable here 🩷</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs25j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1gs04oc</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Need help for tiny nails-need an at home manicure that will last</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gs04oc/need_help_for_tiny_nailsneed_an_at_home_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1gs1hja</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are these cute? Tried something a little different, usually stick to plain French tips </t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hk11ayk5n31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1gs198p</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Buff before or after dehydrating nails for press on nails?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gs198p/buff_before_or_after_dehydrating_nails_for_press/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1gs1250</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French manicure with lilac tips! Gel on natural nail. Thoughts? </t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs1250</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1gs0q12</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Matte red</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eatp7eafh31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1gs0dcx</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Paid fifty bucks for this BIAB - worth it?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sg0cokdre31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1gs003h</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>First time with short nails</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs003h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1grzsot</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>What colour(s) should I wear?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grzsot/what_colours_should_i_wear/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1grzds1</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>New funky nails💖</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grzds1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1grz7cu</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>What nail shape is best?</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grz7cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1grz5ye</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red might be a new fav </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grz5ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1grz1vq</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>New to polish</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1yd0abtl431e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1gryww0</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue jelly nails 🪼 </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hayznuei331e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1gryomi</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I took your advice from yesterday and redid my nails, way more carefully </t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onmsoy4p131e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1grw1z0</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it appropriate to ask for a refund? </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ewmueh0f21e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1grxger</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Tip to make gel manicures last longer</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grxger/tip_to_make_gel_manicures_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1grwfd2</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Skin, Bella </t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grwfd2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1grw9vy</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>November nails</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grw9vy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1grvjy8</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>blue chrome :D</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grvjy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1grvgqy</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>What colour would you say this is ? I did ask for grey but they look pink to me(please ignore the orange hands )😬</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dy8jw47921e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1grv2dq</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>New color ❤️</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dubzgdt2521e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1gruxwl</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Classics ❤️</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9gerqjir321e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1gru1zo</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>New Year Nails 🎉</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1ndmummt11e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1grtv9a</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>First extra long nails</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grtv9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1grtdzf</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Minimal glitter nails</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5ok5zi5l11e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1grt9a1</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Fall Nails</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ncbjgrudj11e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1grt4rv</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">November nails. Frozen style </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grt4rv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1grt22c</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>How can I quit nail biting?</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1grt22c/how_can_i_quit_nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1grsrre</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Current Set</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ctlzatlmc11e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1grrkew</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>I'm embarrassed to show this but I've been doing shellac for about 10 years and now my nails look like this.. The nail is separating from the nail bed and the smile line looks all wonky. Will this ever grow back and be normal again?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fcarn6t5w01e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1grrqeg</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>First attempt making a sweater nails</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grrqeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1gsi934</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>got a little carried away layering</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsi934</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1gshzqo</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about thermals </t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gshzqo/question_about_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1gshue9</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Christmas ideas for the laquerista who has everything.</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gshue9/christmas_ideas_for_the_laquerista_who_has/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1gsha61</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Favorite holiday polish?</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsha61/favorite_holiday_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1gsgl1z</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Just introduced to manicures and have a couple of questions, please!</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsgl1z/just_introduced_to_manicures_and_have_a_couple_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1gsgcyi</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first magnetized mani </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsgcyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1gsg4c1</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Magnetic polish</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsg4c1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1gsfiak</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Sally Hansen "Lavish Lilac" and Essie "Zest Has Yet to Come"</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s5h7vx1z61e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1gsfhfs</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>What’s your favorite red chrome nail polish?</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsfhfs/whats_your_favorite_red_chrome_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1gsf81e</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe for LL Gumption? </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jk21fqowv61e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1gsf6ff</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Looking for recs</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsf6ff/looking_for_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1gse3gn</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>If KBShimmer chips like crazy on you, what other brands also do?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gse3gn/if_kbshimmer_chips_like_crazy_on_you_what_other/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1gsdww9</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Something pink and dreamy 🩷</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/50v1neomi61e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1gsdds9</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>extra long nail lacquer strips</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsdds9/extra_long_nail_lacquer_strips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1gsd0e9</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>In Honor of Neopets' 25th Birthday: Faerie Kadoatie - a custom polish from Red Eyed Lacquer</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsd0e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1gscwbx</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Thank you for the Sally Hansen Insta-Dry recommendation!</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqajt4qc861e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1gsclmf</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Essie Ink Jelly 😍</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsclmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1gscjl9</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails are peeling. Not sure what to do. </t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gscjl9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1gsc8ct</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For those of you who find orly bonder does NOT work for you, which base coat do you like? </t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsc8ct/for_those_of_you_who_find_orly_bonder_does_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1gsc7uv</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Cat Eye!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mo6wxsgw161e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1gsc26x</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zoya Dream - I'm in love! </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsc26x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1gsbxnc</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love a bright ass red </t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5cbol8c5z51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1gsbktz</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Deep maroons for fall? Groundbreaking</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsbktz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1gsbevs</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I used to think it was ragebait but I’m wondering if flooding the cuticle on purpose is just a technique I’m unfamiliar with? Attached example pic from ig reel 😖 </t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9v288ijau51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1gsb8g9</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Cirque Bonbon Jelly vs Holo Taco Devil's Advocate?</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsb8g9/cirque_bonbon_jelly_vs_holo_taco_devils_advocate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1gsahdo</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink is for year round wear, but this one feels more like a fall color </t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsahdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1gsagsd</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>I am FERAL thinking about BKL's Baldur's Gate 3 collection 😭</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsagsd/i_am_feral_thinking_about_bkls_baldurs_gate_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1gsa966</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Please enjoy these various skittle mani experiments over different base colors 😇</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsa966</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1gsa29h</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first ILNP mani- Hex </t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsa29h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1gs9zd3</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>I think I did it! I velveted!</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2wew68fph51e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1gs9qli</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>What is your Niche Interest/fave piece of media that you would like to see be made into nail polish?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gs9qli/what_is_your_niche_interestfave_piece_of_media/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1gs8zej</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Periwinkle with orange shimmer</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wdrw4k5e951e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1gs8byl</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Share photos of your "comfort" nail polish</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xqbijw21451e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1gs84l2</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Flower Child over Black?</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gs84l2/flower_child_over_black/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1gs7x8f</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>looking for colours to match my rings!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gs7x8f/looking_for_colours_to_match_my_rings/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1gs7v89</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Tried another OPI dip powder combo😍😍😍</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3ki283bb051e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1gs7q9f</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Vampy Reds Never Fail 🧛‍♀️</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/grnuvm4az41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1gs7nbx</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Essie Gel Setter Yellowing?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6ogrlyny41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1gs7lra</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>Have you ever dreamt of a better version of yourself?</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs7lra</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1gs6x6w</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top coats? </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gs6x6w/top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1gs6rdg</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Orly Light My (Camp)fire 🔥</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs6rdg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1gs6a9q</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Need help (Sorry if this is the wrong place)</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gs6a9q/need_help_sorry_if_this_is_the_wrong_place/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1gs624i</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">An unhealthy obsession with reflective polishes was born today. </t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs624i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1gs5bhd</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Garden Path Lacquers Blessed with Beauty and Rage</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sywocv47g41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1gs576i</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help me pick my next color! </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gs576i/help_me_pick_my_next_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1gs3m7p</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>In love with this (potential) prugly</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs3m7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1gs3ctg</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>When movie night and nail night intersect</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs3ctg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1gs34zr</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Bubble lumpies?</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i342j12hz31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1gs2ow8</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Gel removal disaster :(</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tvznoa3w31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1gs2i3a</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>otherworldly ✨</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs2i3a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1gs2fhj</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>very proud of my celestial set ✨</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x2bojg8u31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1gs1nu4</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Emerald recs like this, but with chunky glitter instead of holo</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ont05rcgo31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1gs1ge5</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Woodland Animals 🦡</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6x5cnyrwm31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1gs1ddy</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue to black feels appropriate </t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/860ork48m31e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1gs163p</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>We Have "Which Witch" At Home</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs163p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1gs0d3p</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Feeling blue, vibing with this color</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2l34jepe31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1gs08qh</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cart help </t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs08qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1grzu61</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Experimented with colours, juicy euphoric.</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grzu61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1grzlum</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Anyone know of a copper speckled polish like G&amp;G’s friends and family but in a clear base?</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grzlum</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1grypv5</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue and Gold never gets old, s’what I always say </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5i2ke5z131e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1gryexl</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Temperatures are *finally* below 50 degrees here, so I did the thing🖤❤️</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rstugu2fz21e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1grxnbd</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>ILNP Starlight</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d6w8bd5t21e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1grxkab</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I got through so many polishes in October! </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grxkab</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1gruv0j</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>After spending way too much time and money trying to view the Northern Lights, I recreated them on my nails instead</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/v6Nm95f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1grtdot</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Seche Vive is NOT worth it</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grtdot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1grssur</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any chance someone has a comparison between ILNP Tidal wave and EDM Deafening Silence? </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1grssur/any_chance_someone_has_a_comparison_between_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1grrr7m</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t xml:space="preserve">loving these blue green jellies </t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3fvvk4my01e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1gsg0if</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Interesting present for friend who’s super into nail art?</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gsg0if/interesting_present_for_friend_whos_super_into/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1gse55m</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Fall nails</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gse55m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1gse35k</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some of my work over the past few years </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gse35k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1gse2me</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Work in Progress</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gse2me</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1gsd51h</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Blue celestial cat eye 😍</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bvlxzv1ma61e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1gsbwox</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>it’s the most wonderful time of the year 🎅</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3yl4c4wy51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1gsbu9o</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blue jelly nails 🪼 </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rdezku8y51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1gs9uf2</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i got a little carried away </t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs9uf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1gs9frp</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Did these nails</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7ogfju5d51e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1gs7x9q</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Golden flowers 👌😊</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/334gbfkt051e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1gs7obj</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Made this set of geode like press ons</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs7obj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1gs7fs1</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Uzumaki 🌀 Junji Ito Nails</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs7fs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1gs6vrj</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Trying out spinning charms</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2sq0gvbns41e1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1gs61ki</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>My hair appointment got canceled and I was bored soooo….</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boiwoxl1m41e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1gs582o</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Go easy on me!</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gs582o/go_easy_on_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1gs2tf0</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>How to we feel about this? 🎄✨</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9cbd8651x31e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1gs0y1m</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">It’s been a while ✨ </t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gs0y1m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1grytl1</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>how do we feel about these ?🍵✨</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1grytl1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1gru2c3</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Descendants 4 inspired nails</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gru2c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1gru1sh</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>New Year Nails 🎉</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cytbp81kt11e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1grsre2</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hearts </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zkw05hgc11e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Nov 17 08:09:49 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_11_17.xlsx
+++ b/data/collected_data/2024_11_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1198"/>
+  <dimension ref="A1:C1378"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20800,6 +20800,3066 @@
         </is>
       </c>
     </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1gt8oj5</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>gel nails lifting at the base when applying</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt8oj5/gel_nails_lifting_at_the_base_when_applying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1gt8o06</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Nude Pink for fall</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5eowpc63f1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1gt86nc</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pushed back my cuticles and this happened instead 🥲 can i deal with this without cutting my cuticles? </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0xvi6cwwe1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1gt86i8</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>My Melody &amp; Hello Kitty 🎀</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt86i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1gt7qmq</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>I just wanted to throw my blue metallics up here too</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qnz1jj7re1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1gt7q99</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails night out! </t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gb4gv3v6re1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1gt7do0</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I absolutely love this cat eye gel! </t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt7do0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1gt7azs</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beautiful </t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmpgz41vle1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1gt6lf0</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Gel X cut out heart 💝</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zpjbm3iide1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1gt6jjt</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>What do we think?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt6jjt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1gt6jgr</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>My best set so far</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dn0hj4nwce1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1gt6i5i</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art 😅 any advice?</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt6i5i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1gt6i3a</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Attempted an ombre glitter tip</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xf96e9qgce1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1gt6cet</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Best Fall Nail Color?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt6cet/best_fall_nail_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1gt5vzx</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>16 Year old Nail Tech</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt5vzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1gt56lt</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>What's the best nail polish top coat?</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt56lt/whats_the_best_nail_polish_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1gt1euw</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Was finally able to grow out my nails after quitting my 10 year nanny career. Took the first photo yesterday as a flex. Broke my middle nail opening a door this morning. That’s what I get for bragging. </t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt1euw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1gt01ns</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Press on suggestions?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt01ns/press_on_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1gsypa0</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Nail question: extensions ?</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsypa0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1gt4v20</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Festive Nails🎄</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt4v20</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1gt1t1i</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Artists in St. Petersburg/Tampa area??</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt1t1i/artists_in_st_petersburgtampa_area/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1gszlwh</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Best liquid latex?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gszlwh/best_liquid_latex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1gt3zr6</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Lifelong nail biter- need some help</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt3zr6/lifelong_nail_biter_need_some_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1gt48ie</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some berry brightness ⭐️🍓🍒on this rainy day </t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbq1030mod1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1gt3yp7</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt3yp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1gt3ukc</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nothing fancy but really loving them. </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/svb04zfukd1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1gt3r85</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t xml:space="preserve">picking the wrong color </t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt3r85/picking_the_wrong_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1gt2oek</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wicked </t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwqkshtj9d1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1gt2j04</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Need suggestions of shape!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt2j04</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1gt27wq</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>interview on monday but my nail set isn't very "professional"</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt27wq/interview_on_monday_but_my_nail_set_isnt_very/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1gt277f</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>chocolate bonbon nails ! 🥹🍫 (I'm a begginer hobbyist practicing, any tips and tricks welcomed!)</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqibtpw25d1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1gt243l</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>My first dip nails with tips.</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt243l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1gt21r0</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Let the holiday nails commence 🌲 </t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2rwy9np3d1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1gt1z2g</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>My nail tech never disappoints</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt1z2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1gt1elg</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Nails of the week 💅🏾✨</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lynv69eqxc1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1gt111b</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Dupe for King Midas?</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gt111b/dupe_for_king_midas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1gt0mwu</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>My second mani ever ❤️</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt0mwu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1gt0lrx</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>help!</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ka6nvudxqc1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1gt0k3t</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Colder days call for blue</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt0k3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1gt0dmp</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New press ons </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt0dmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1gt01f5</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude set </t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rljke0gzlc1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1gszqcb</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nail artist </t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gszqcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1gsz9q5</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>November nails</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jxtvescfc1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1gsynkj</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Strawberry milks x2</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67f912h2ac1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1gsyh8u</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Fall blend!🍁</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsyh8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1gsy1o8</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Does this length/shape suit me?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsy1o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1gsxcnt</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Does anyone know why this nail does this? None of my others do. Lol (Artistic rendition at the end)</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsxcnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1gsxhhd</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Can’t stop doing textured stripes</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eyrnrki90c1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1gsx4q4</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What does my nail girl need to do differently? </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsx4q4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1gswbuy</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64v0dm5kqb1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1gsw8rc</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I miss my glorious nails </t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vlqkucupb1e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1gsvx0w</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm obsessed with this holographic chrome powder </t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/saiun6o3nb1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1gsvw8i</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Sunflowers</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qx0sdo1xmb1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1gsvo22</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ballerina nails </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsvo22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1gsv0yp</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>tried 3d gel for first time</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10xg3k1pfb1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1gsuvrs</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Obsessed with this blue</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s41bsmajeb1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1gstgmh</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Went almond for the first time!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gstgmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1gst7cj</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why do the corners of my thumbs always split!? </t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gst7cj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1gsujmq</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Winter nails❄️ and the first time square, I'm in love💖</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6su92btbb1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1gssora</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible to acrylic applied without the fake tips? </t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gssora</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1gss6oi</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>For my vampire costume</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gss6oi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1gsu0x4</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Red ❤️❤️❤️</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5baznldn7b1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1gstsks</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are yalls thoughts on my nails (done by a professional) </t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixbs1meu5b1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1gstk31</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>short &amp; soft pink 🩷✨</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gstk31</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1gst6fv</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>This is literally... the cutest set I've ever done (⁠*⁠´⁠ω⁠｀⁠*⁠)</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gst6fv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1gst6b3</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>My second set of nails I’m so happy</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgtmrv9x0b1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1gst1wn</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail lamp recommendations </t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gst1wn/nail_lamp_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1gst0hh</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Caramel nails </t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnlladujza1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1gssrkk</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>🔮💜♍️</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c62vhf5mxa1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1gsskz3</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>How do they look?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsskz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1gssbv6</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>One of my favourite nail sets ever.</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/e32at2o1ua1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1gss12g</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Nude autumn set - mani pedi matched</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gss12g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1gsruvw</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Fall Butterfly🦋🧡</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsruvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1gsrmzf</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Crazy what a few months can do</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wb5rdunhoa1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1gsrl6k</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple and minimal </t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1175o744oa1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1gsrhc6</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>New claws and I’m in love</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsrhc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1gsr6ci</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>I need some serious advice!</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gsr6ci/i_need_some_serious_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1gsqwr0</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>First DIY GelX set 🩵🎀</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsqwr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1gsqptg</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>🌈 Colorful Nail Design 🌈</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zn7ygduxga1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1gsq4ca</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Almost done growing out damage</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsq4ca</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1gsq8k6</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My wife generally does her nails for the holiday of the month. </t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d26q86s2da1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1gspqnv</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh set ♥️ </t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gspqnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1gsj8qn</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>{Question] How long should I wait between getting new gel nails?</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gsj8qn/question_how_long_should_i_wait_between_getting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1gskn8a</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my nails done and it's my fault I don't like them. </t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gskn8a/got_my_nails_done_and_its_my_fault_i_dont_like/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1gsow0l</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Do my press ons look ok?</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsow0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1gsp0pu</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>😻✨</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i07txq0u2a1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1gsnsq0</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand usually gets nicked during Russian manicure. Can I request to not get dead skin removed? </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gsnsq0/hand_usually_gets_nicked_during_russian_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1gsneft</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand painted Powerpuff Girls </t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsneft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1gsnbia</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Beginner at nail art</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsnbia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1gsn7ep</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Love these press ons</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldhxnbp0m91e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1gsn60t</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>3D Gel X</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsn60t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1gsn5n7</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>My fave colour :)</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipul19xjl91e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1gsn5dg</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Going for a wholesome occult mom vibe 🖤</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qmi5f7tgl91e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1gsmjoz</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Aurora Pigments turn everything white</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1gsmjoz/aurora_pigments_turn_everything_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1gsm34i</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t xml:space="preserve">whimsigoth bday nails !!! </t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onb12gkz991e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1gslv6l</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my red nails </t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gslv6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1gslrwt</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Press on help</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gslrwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1gslfk5</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail is breaking off low down at the pink part! What should I do!? It icks me out! </t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nj8kv3z191e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1gsl64q</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should I change my artist? </t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hybmvj1ly81e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1gskvxo</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>I did my nails today!</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gskvxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1gt8uy7</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Is this a good polish?</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3104cjqo5f1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1gt8hmb</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>mad hatter and ilnp deep space</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gt8hmb/mad_hatter_and_ilnp_deep_space/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1gt7j3j</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>✨shimmer✨</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt7j3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1gt6z3o</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>The ILNP Deep Space experience</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt6z3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1gt69l5</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shadow Lake dupe? </t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aomeg46u9e1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1gt65gg</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Super flashy blue glitter polish?!?</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt65gg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1gt4e3p</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>love love how they came out 💚🌲🥰</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p126cp48qd1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1gt4dd5</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Flower child as a topper is gorgeous</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqj2ttv0qd1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1gt4874</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Experimenting with French </t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt4874</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1gt3qsj</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Mishipeshu-The Great Lynx - LynBDesigns</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt3qsj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1gt36ts</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Had some fun with river styx a couple manis back 🫧🩵</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt36ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1gt2tj3</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>New Cirque order came in after a long week at work</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt2tj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1gt2ci5</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Holo Taco Underglow Collection?</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gt2ci5/holo_taco_underglow_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1gt1zja</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Otherworldly</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt1zja</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1gt1qn9</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I feel them catching on things constantly? </t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hb0tk3z0d1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1gt1k3o</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Bloody Mary</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dq5xag89zc1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1gt1ixo</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>I think she likes this color</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt1ixo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1gt1fq6</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce ✨ Here Kitty Kitty</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt1fq6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1gt0jjc</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>The latest set I’ve done ⛓️🩸</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt0jjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1gszc3e</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I like to match my nails with my clothes! </t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xancalvwfc1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1gsz09y</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Fell in Love With an Oops</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsz09y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1gsytha</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Textured polish! I’m unsure!</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsytha</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1gsydwb</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>holo taco underglow - quick swatches (pr)</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fto5t76s7c1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1gsyc0j</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Forgive me for ignoring this polish in my collection for too long 🙏🏻</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsyc0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1gsy8vs</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Praise the Dog</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsy8vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1gsy557</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Nail Polish trends</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsy557/nail_polish_trends/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1gsy2e2</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Mooncat lunar sale is coming next week. What are your mooncat favorites?</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsy2e2/mooncat_lunar_sale_is_coming_next_week_what_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1gsxhi5</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Swatch Comparison: My five bluest blues on a rainy day</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bx3zae090c1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1gsxgcl</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Recs for Polish Gift Box</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsxgcl/recs_for_polish_gift_box/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1gsx8wb</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cactus </t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsx8wb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1gswsg9</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Does Holo Taco usually do a Black Friday sale?</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gswsg9/does_holo_taco_usually_do_a_black_friday_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1gsvh9i</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Trying out holiday polishes this weekend! 🎄</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxigm0fhjb1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1gsusz9</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Skittle!</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9a124tcwdb1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1gsuatz</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>RIP 🫡</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/79ixh0zv9b1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1gsu8ds</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Essie - Angora Cardi</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsu8ds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1gsttnf</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Vitamin Glow by Holo Taco (pr)</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsttnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1gstnjq</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Going green😍</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gstnjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1gsthnj</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Cirque Folie a Deux</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsthnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1gstgl8</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>nails for a concert!</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a4z3k2h73b1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1gstfa8</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Cirque Tahitian Pearl</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gstfa8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1gst06j</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Mooncat Skittle!</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jt9topbhza1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1gsswks</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>It's time...</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xcakqycqya1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1gsspws</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>To Teach Us About Our Past</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsspws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1gssdtw</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Dark red/brown holo/glitter polish?</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gssdtw/dark_redbrown_hologlitter_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1gsruu9</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cross post: looking for the perfect nude </t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsruu9/cross_post_looking_for_the_perfect_nude/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1gsrip0</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Outer ring on mani</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsrip0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1gsr4s1</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Game changer for nail care?</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsr4s1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1gsqvav</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Just another Deep Space appreciation post</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsqvav</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1gsqg61</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Amazing low light topper</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsqg61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1gsq59m</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>My first holo 😍</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsq59m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1gsq4ee</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Nocturno 🌙</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsq4ee</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1gsq24t</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Obsessed with my vacay shade</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsq24t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1gspyd0</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>New favorite thing: Reversing the skittle on the other hand</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gspyd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1gsplyn</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Does a (non)acid primer under regular nail polish make sense?</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gsplyn/does_a_nonacid_primer_under_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1gsoklt</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Still feeling the warm orange autumn vibes 🍂 </t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dox9svhuy91e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1gsnuh1</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>The perfect rose gold chrome doesn't exi...</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsnuh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1gsn5tt</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Matching the Fuji countryside 🍂</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsn5tt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1gsmr3z</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Catrice in shade 100 Party Animal</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4xhfz2jh91e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1gskrlu</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>ILNP pros, I'm desperate</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gskrlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1gskdes</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Do I just have to bite the bullet and try out top coats?</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1gskdes/do_i_just_have_to_bite_the_bullet_and_try_out_top/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1gsk0bh</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Mooncat - Fields of Lavender</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lhulw149i81e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1gsjce1</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Mooncat - Fields of Lavender</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsjb8e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1gsey35</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>green &amp; black velvet ✨</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b81aahtus61e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1gt4vgm</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Simple Minimal Tortoise Shell Set hand painted by me :)</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0tu412vud1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1gt3deu</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Ignore messy cuticle lol</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1cozky5gd1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1gt34ww</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Meow✨🐱👁️</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gt34ww</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1gt0vy7</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First after Halloween fall set </t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldzgdz1etc1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1gszbz1</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Gingerbread vibes</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gszbz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1gsyein</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Can I first do art on soft gel tips and then apply it on my nail when I want to?</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1gsyein/can_i_first_do_art_on_soft_gel_tips_and_then/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1gsw9z0</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Fall Baby Shower Nails For My Best Friend 🩷</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsw9z0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1gstnzg</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Beetlejuice 🥰</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02cj4siu4b1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1gsti62</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Mutated💎</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mggcfpj3b1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1gsthrp</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Yes, its green💚</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8rk4hjac3b1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1gstgco</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Evil Snowflake❄️</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rnvizqhy2b1e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1gssknj</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Cat &amp; Rabbit</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gssknj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1gsrzlf</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Nude autumn set- mani pedi matched</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1gsrzlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1gsqtv5</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Evil eye 🧿</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oi5gxgsuha1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1gsqpje</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>🌈 Colorful Nail Design 🌈</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h4fq8znvga1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1gsps6z</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sad to change these. </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31n4w6na9a1e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1gpkxp5</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Becoming OBSESSED with painting pumpkins on my nails</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtvst9hz4h0e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>